<commit_message>
Result simulation & Sensitivity
</commit_message>
<xml_diff>
--- a/js_simulation/simulation_results_v1000.xlsx
+++ b/js_simulation/simulation_results_v1000.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,16 +510,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9834140176700991</v>
+        <v>0.9834224325798011</v>
       </c>
       <c r="D2" t="n">
-        <v>121489.4720318987</v>
+        <v>121829.664114389</v>
       </c>
       <c r="E2" t="n">
-        <v>125868.3226974954</v>
+        <v>126318.9527286087</v>
       </c>
       <c r="F2" t="n">
-        <v>121489.4720318987</v>
+        <v>121829.664114389</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -527,10 +527,10 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>121489.4720318987</v>
+        <v>121829.664114389</v>
       </c>
       <c r="K2" t="n">
-        <v>125868.3226974954</v>
+        <v>126318.9527286087</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -548,16 +548,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.8225853631425034</v>
+        <v>0.8229241532103124</v>
       </c>
       <c r="D3" t="n">
-        <v>186233.2080458938</v>
+        <v>187893.2467576699</v>
       </c>
       <c r="E3" t="n">
-        <v>194987.4256253544</v>
+        <v>197091.1653749209</v>
       </c>
       <c r="F3" t="n">
-        <v>186233.2080458938</v>
+        <v>187893.2467576699</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -565,10 +565,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>186233.2080458938</v>
+        <v>187893.2467576699</v>
       </c>
       <c r="K3" t="n">
-        <v>194987.4256253544</v>
+        <v>197091.1653749209</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
@@ -586,16 +586,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.6473226753526866</v>
+        <v>0.6484745352049633</v>
       </c>
       <c r="D4" t="n">
-        <v>199551.9300674134</v>
+        <v>198985.6758993856</v>
       </c>
       <c r="E4" t="n">
-        <v>208883.8864548269</v>
+        <v>208547.70366944</v>
       </c>
       <c r="F4" t="n">
-        <v>199551.9300674134</v>
+        <v>198985.6758993856</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
@@ -603,10 +603,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>199551.9300674134</v>
+        <v>198985.6758993856</v>
       </c>
       <c r="K4" t="n">
-        <v>208883.8864548269</v>
+        <v>208547.70366944</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -624,16 +624,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4166960715997488</v>
+        <v>0.419118657227098</v>
       </c>
       <c r="D5" t="n">
-        <v>209997.9724065157</v>
+        <v>211240.7588842058</v>
       </c>
       <c r="E5" t="n">
-        <v>218520.1047617262</v>
+        <v>220353.420098644</v>
       </c>
       <c r="F5" t="n">
-        <v>209997.9724065157</v>
+        <v>211240.7588842058</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
@@ -641,10 +641,10 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>209997.9724065157</v>
+        <v>211240.7588842058</v>
       </c>
       <c r="K5" t="n">
-        <v>218520.1047617262</v>
+        <v>220353.420098644</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -653,43 +653,39 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>STO 15%</t>
+          <t>Trad PF</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Perfect (100%)</t>
+          <t>Extreme (15%)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9823143022526057</v>
+        <v>0.4044718914155936</v>
       </c>
       <c r="D6" t="n">
-        <v>17233.06405730591</v>
+        <v>211331.4606634509</v>
       </c>
       <c r="E6" t="n">
-        <v>21190.57548278707</v>
+        <v>219667.2774161219</v>
       </c>
       <c r="F6" t="n">
-        <v>17233.06405730591</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
+        <v>211331.4606634509</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>324.2426528223837</v>
+        <v>211331.4606634509</v>
       </c>
       <c r="K6" t="n">
-        <v>363.9387099913973</v>
+        <v>219667.2774161219</v>
       </c>
       <c r="L6" t="n">
-        <v>-16908.82140448353</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -700,38 +696,38 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Good (84%)</t>
+          <t>Perfect (100%)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.81875756094707</v>
+        <v>0.9822986308332026</v>
       </c>
       <c r="D7" t="n">
-        <v>127259.3429977431</v>
+        <v>17945.48087318345</v>
       </c>
       <c r="E7" t="n">
-        <v>135722.365120862</v>
+        <v>21983.47267458183</v>
       </c>
       <c r="F7" t="n">
-        <v>127259.3429977431</v>
+        <v>17945.48087318345</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0001010327839969894</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>2811.405402306351</v>
+        <v>17945.48087318345</v>
       </c>
       <c r="K7" t="n">
-        <v>3161.167102612039</v>
+        <v>21983.47267458183</v>
       </c>
       <c r="L7" t="n">
-        <v>-124447.9375954367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -742,38 +738,38 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Recession (65%)</t>
+          <t>Good (84%)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6416063235468267</v>
+        <v>0.8186366174467081</v>
       </c>
       <c r="D8" t="n">
-        <v>139668.8077281435</v>
+        <v>126819.6940210681</v>
       </c>
       <c r="E8" t="n">
-        <v>149294.3209779384</v>
+        <v>136490.3980208867</v>
       </c>
       <c r="F8" t="n">
-        <v>139668.8077281435</v>
+        <v>126819.6940210681</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0005745609146250596</v>
+        <v>7.707580972188864e-05</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>6113.141504233423</v>
+        <v>126819.6940210681</v>
       </c>
       <c r="K8" t="n">
-        <v>6771.035511468657</v>
+        <v>136557.8393543933</v>
       </c>
       <c r="L8" t="n">
-        <v>-133555.6662239101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -784,122 +780,122 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Crisis (41%)</t>
+          <t>Recession (65%)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4136345003583995</v>
+        <v>0.6416906222967823</v>
       </c>
       <c r="D9" t="n">
-        <v>156576.5980458368</v>
+        <v>140495.7561256773</v>
       </c>
       <c r="E9" t="n">
-        <v>167496.3367301368</v>
+        <v>149716.8516460881</v>
       </c>
       <c r="F9" t="n">
-        <v>156576.5980458368</v>
+        <v>140495.7561256773</v>
       </c>
       <c r="G9" t="n">
-        <v>0.009999999999999905</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.02320890123150835</v>
+        <v>0.0006071513183129611</v>
       </c>
       <c r="I9" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>11477.75481791698</v>
+        <v>140495.7561256773</v>
       </c>
       <c r="K9" t="n">
-        <v>12798.5764749229</v>
+        <v>149883.7387885563</v>
       </c>
       <c r="L9" t="n">
-        <v>-145098.8432279198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>STO 28%</t>
+          <t>STO 15%</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Perfect (100%)</t>
+          <t>Crisis (41%)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.982289528511714</v>
+        <v>0.413327534293121</v>
       </c>
       <c r="D10" t="n">
-        <v>17395.12467039677</v>
+        <v>156402.8011420401</v>
       </c>
       <c r="E10" t="n">
-        <v>21038.2149648252</v>
+        <v>166524.1210733571</v>
       </c>
       <c r="F10" t="n">
-        <v>17395.12467039677</v>
+        <v>156402.8011420401</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.009999999999999905</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.02749445546428887</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="J10" t="n">
-        <v>323.2820483378213</v>
+        <v>156507.8011420401</v>
       </c>
       <c r="K10" t="n">
-        <v>365.8460643810284</v>
+        <v>167021.1796536501</v>
       </c>
       <c r="L10" t="n">
-        <v>-17071.84262205895</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>STO 28%</t>
+          <t>STO 15%</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Good (84%)</t>
+          <t>Extreme (15%)</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.8169322596973189</v>
+        <v>0.3967631143114563</v>
       </c>
       <c r="D11" t="n">
-        <v>111465.1348523069</v>
+        <v>159597.0649230403</v>
       </c>
       <c r="E11" t="n">
-        <v>120002.435093471</v>
+        <v>168045.213339946</v>
       </c>
       <c r="F11" t="n">
-        <v>111465.1348523069</v>
+        <v>159597.0649230403</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.009999999999999905</v>
       </c>
       <c r="H11" t="n">
-        <v>4.535532507098437e-05</v>
+        <v>0.02485180089578153</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="J11" t="n">
-        <v>2930.038027836275</v>
+        <v>159702.0649230403</v>
       </c>
       <c r="K11" t="n">
-        <v>3257.968593530237</v>
+        <v>168454.7530164294</v>
       </c>
       <c r="L11" t="n">
-        <v>-108535.0968244706</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12">
@@ -910,38 +906,38 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Recession (65%)</t>
+          <t>Perfect (100%)</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6390038704741831</v>
+        <v>0.9823196459810106</v>
       </c>
       <c r="D12" t="n">
-        <v>125142.6105336513</v>
+        <v>17154.89126112844</v>
       </c>
       <c r="E12" t="n">
-        <v>134675.7722791967</v>
+        <v>20601.66407879172</v>
       </c>
       <c r="F12" t="n">
-        <v>125142.6105336513</v>
+        <v>17154.89126112844</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0005201782828060917</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>6315.191813822651</v>
+        <v>17154.89126112844</v>
       </c>
       <c r="K12" t="n">
-        <v>6957.46729829272</v>
+        <v>20601.66407879172</v>
       </c>
       <c r="L12" t="n">
-        <v>-118827.4187198286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -952,164 +948,164 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Crisis (41%)</t>
+          <t>Good (84%)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.4132660348296509</v>
+        <v>0.8171811642575961</v>
       </c>
       <c r="D13" t="n">
-        <v>143094.331373237</v>
+        <v>111529.9940324439</v>
       </c>
       <c r="E13" t="n">
-        <v>152803.629663798</v>
+        <v>120129.3880140484</v>
       </c>
       <c r="F13" t="n">
-        <v>143094.331373237</v>
+        <v>111529.9940324439</v>
       </c>
       <c r="G13" t="n">
-        <v>0.00999999999999995</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0234222611596614</v>
+        <v>5.912561875968674e-05</v>
       </c>
       <c r="I13" t="n">
-        <v>196</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>11574.67257200867</v>
+        <v>111529.9940324439</v>
       </c>
       <c r="K13" t="n">
-        <v>12617.30770145806</v>
+        <v>120217.1805994794</v>
       </c>
       <c r="L13" t="n">
-        <v>-131519.6588012284</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>STO 40%</t>
+          <t>STO 28%</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Perfect (100%)</t>
+          <t>Recession (65%)</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.9823121013038794</v>
+        <v>0.6396710372473863</v>
       </c>
       <c r="D14" t="n">
-        <v>16948.71173573424</v>
+        <v>125263.9032285218</v>
       </c>
       <c r="E14" t="n">
-        <v>20564.07821330571</v>
+        <v>135025.4596369151</v>
       </c>
       <c r="F14" t="n">
-        <v>16948.71173573424</v>
+        <v>125263.9032285218</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>0.000555384797919084</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>318.4910569569728</v>
+        <v>125263.9032285218</v>
       </c>
       <c r="K14" t="n">
-        <v>356.4227330958275</v>
+        <v>135269.5300862248</v>
       </c>
       <c r="L14" t="n">
-        <v>-16630.22067877727</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>STO 40%</t>
+          <t>STO 28%</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Good (84%)</t>
+          <t>Crisis (41%)</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.8155323903846202</v>
+        <v>0.4119103335077707</v>
       </c>
       <c r="D15" t="n">
-        <v>98844.58605678441</v>
+        <v>143370.4323154436</v>
       </c>
       <c r="E15" t="n">
-        <v>107130.037330868</v>
+        <v>153551.0916585604</v>
       </c>
       <c r="F15" t="n">
-        <v>98844.58605678441</v>
+        <v>143370.4323154436</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>0.00999999999999995</v>
       </c>
       <c r="H15" t="n">
-        <v>5.003315759281891e-05</v>
+        <v>0.02489130257355281</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="J15" t="n">
-        <v>3058.693908051168</v>
+        <v>143566.4323154436</v>
       </c>
       <c r="K15" t="n">
-        <v>3368.927032756765</v>
+        <v>154280.4359803746</v>
       </c>
       <c r="L15" t="n">
-        <v>-95785.89214873324</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>STO 40%</t>
+          <t>STO 28%</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Recession (65%)</t>
+          <t>Extreme (15%)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.6368769188635667</v>
+        <v>0.3939539599978985</v>
       </c>
       <c r="D16" t="n">
-        <v>115089.4501373783</v>
+        <v>145775.4276440667</v>
       </c>
       <c r="E16" t="n">
-        <v>124018.9028566052</v>
+        <v>154961.0768302313</v>
       </c>
       <c r="F16" t="n">
-        <v>115089.4501373783</v>
+        <v>145775.4276440667</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>0.00999999999999995</v>
       </c>
       <c r="H16" t="n">
-        <v>0.000422501511520011</v>
+        <v>0.02332944757897115</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="J16" t="n">
-        <v>6530.712254235763</v>
+        <v>145971.4276440667</v>
       </c>
       <c r="K16" t="n">
-        <v>7185.912309762005</v>
+        <v>155692.106488982</v>
       </c>
       <c r="L16" t="n">
-        <v>-108558.7378831425</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17">
@@ -1120,38 +1116,206 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>Perfect (100%)</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.9823392407637377</v>
+      </c>
+      <c r="D17" t="n">
+        <v>17438.78386417262</v>
+      </c>
+      <c r="E17" t="n">
+        <v>21352.25180847063</v>
+      </c>
+      <c r="F17" t="n">
+        <v>17438.78386417262</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>17438.78386417262</v>
+      </c>
+      <c r="K17" t="n">
+        <v>21352.25180847063</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Good (84%)</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8154540468899483</v>
+      </c>
+      <c r="D18" t="n">
+        <v>97988.6364167962</v>
+      </c>
+      <c r="E18" t="n">
+        <v>107144.728420625</v>
+      </c>
+      <c r="F18" t="n">
+        <v>97988.6364167962</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>5.212294998329787e-05</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>97988.6364167962</v>
+      </c>
+      <c r="K18" t="n">
+        <v>107233.7188230355</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Recession (65%)</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.637036077665824</v>
+      </c>
+      <c r="D19" t="n">
+        <v>113193.7073697877</v>
+      </c>
+      <c r="E19" t="n">
+        <v>123025.4694082533</v>
+      </c>
+      <c r="F19" t="n">
+        <v>113193.7073697877</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.0004304157314349371</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>113193.7073697877</v>
+      </c>
+      <c r="K19" t="n">
+        <v>123325.2614599991</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>Crisis (41%)</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>0.4094635588208302</v>
-      </c>
-      <c r="D17" t="n">
-        <v>131034.2677424282</v>
-      </c>
-      <c r="E17" t="n">
-        <v>141460.4748809713</v>
-      </c>
-      <c r="F17" t="n">
-        <v>131034.2677424282</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.009369397213637195</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.02533414121601242</v>
-      </c>
-      <c r="I17" t="n">
-        <v>262.3431219818424</v>
-      </c>
-      <c r="J17" t="n">
-        <v>11643.08994277793</v>
-      </c>
-      <c r="K17" t="n">
-        <v>12674.35080814071</v>
-      </c>
-      <c r="L17" t="n">
-        <v>-119391.1777996503</v>
+      <c r="C20" t="n">
+        <v>0.4112745638097692</v>
+      </c>
+      <c r="D20" t="n">
+        <v>131654.3383120974</v>
+      </c>
+      <c r="E20" t="n">
+        <v>142258.0594928669</v>
+      </c>
+      <c r="F20" t="n">
+        <v>131654.3383120974</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.006437157214779519</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.02494204968688549</v>
+      </c>
+      <c r="I20" t="n">
+        <v>180.2404020138272</v>
+      </c>
+      <c r="J20" t="n">
+        <v>131834.5787141112</v>
+      </c>
+      <c r="K20" t="n">
+        <v>142956.4368840997</v>
+      </c>
+      <c r="L20" t="n">
+        <v>180.2404020138272</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Extreme (15%)</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.3921787635140916</v>
+      </c>
+      <c r="D21" t="n">
+        <v>135250.7601474534</v>
+      </c>
+      <c r="E21" t="n">
+        <v>145073.068370846</v>
+      </c>
+      <c r="F21" t="n">
+        <v>135250.7601474534</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.009999999999999966</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.02361353547521183</v>
+      </c>
+      <c r="I21" t="n">
+        <v>280</v>
+      </c>
+      <c r="J21" t="n">
+        <v>135530.7601474534</v>
+      </c>
+      <c r="K21" t="n">
+        <v>146081.5939024307</v>
+      </c>
+      <c r="L21" t="n">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -1165,7 +1329,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1242,19 +1406,19 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>121489.4720318987</v>
+        <v>121829.664114389</v>
       </c>
       <c r="E2" t="n">
-        <v>125868.3226974954</v>
+        <v>126318.9527286087</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>121489.4720318987</v>
+        <v>121829.664114389</v>
       </c>
       <c r="H2" t="n">
-        <v>125868.3226974954</v>
+        <v>126318.9527286087</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1280,19 +1444,19 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>186233.2080458938</v>
+        <v>187893.2467576699</v>
       </c>
       <c r="E3" t="n">
-        <v>194987.4256253544</v>
+        <v>197091.1653749209</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>186233.2080458938</v>
+        <v>187893.2467576699</v>
       </c>
       <c r="H3" t="n">
-        <v>194987.4256253544</v>
+        <v>197091.1653749209</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -1318,19 +1482,19 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>199551.9300674134</v>
+        <v>198985.6758993856</v>
       </c>
       <c r="E4" t="n">
-        <v>208883.8864548269</v>
+        <v>208547.70366944</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>199551.9300674134</v>
+        <v>198985.6758993856</v>
       </c>
       <c r="H4" t="n">
-        <v>208883.8864548269</v>
+        <v>208547.70366944</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -1356,19 +1520,19 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>209997.9724065157</v>
+        <v>211240.7588842058</v>
       </c>
       <c r="E5" t="n">
-        <v>218520.1047617262</v>
+        <v>220353.420098644</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>209997.9724065157</v>
+        <v>211240.7588842058</v>
       </c>
       <c r="H5" t="n">
-        <v>218520.1047617262</v>
+        <v>220353.420098644</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -1380,45 +1544,45 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>STO 15%_Perfect</t>
+          <t>Trad PF_Extreme</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>STO 15%</t>
+          <t>Trad PF</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Perfect (100%)</t>
+          <t>Extreme (15%)</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>17233.06405730591</v>
+        <v>211331.4606634509</v>
       </c>
       <c r="E6" t="n">
-        <v>21190.57548278707</v>
+        <v>219667.2774161219</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>324.2426528223837</v>
+        <v>211331.4606634509</v>
       </c>
       <c r="H6" t="n">
-        <v>363.9387099913973</v>
+        <v>219667.2774161219</v>
       </c>
       <c r="I6" t="n">
-        <v>-16908.82140448353</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>-98.11848518786813</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>STO 15%_Good</t>
+          <t>STO 15%_Perfect</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1428,35 +1592,35 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Good (84%)</t>
+          <t>Perfect (100%)</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>127259.3429977431</v>
+        <v>17945.48087318345</v>
       </c>
       <c r="E7" t="n">
-        <v>135722.365120862</v>
+        <v>21983.47267458183</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2811.405402306351</v>
+        <v>327.9697713389484</v>
       </c>
       <c r="H7" t="n">
-        <v>3161.167102612039</v>
+        <v>363.3328414879439</v>
       </c>
       <c r="I7" t="n">
-        <v>-124447.9375954367</v>
+        <v>-17617.5111018445</v>
       </c>
       <c r="J7" t="n">
-        <v>-97.79080628888975</v>
+        <v>-98.17241023711411</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>STO 15%_Recession</t>
+          <t>STO 15%_Good</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1466,35 +1630,35 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Recession (65%)</t>
+          <t>Good (84%)</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>139668.8077281435</v>
+        <v>126819.6940210681</v>
       </c>
       <c r="E8" t="n">
-        <v>149294.3209779384</v>
+        <v>136490.3980208867</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>6113.141504233423</v>
+        <v>2759.67069166779</v>
       </c>
       <c r="H8" t="n">
-        <v>6771.035511468657</v>
+        <v>3111.757681282013</v>
       </c>
       <c r="I8" t="n">
-        <v>-133555.6662239101</v>
+        <v>-124060.0233294003</v>
       </c>
       <c r="J8" t="n">
-        <v>-95.62311613905069</v>
+        <v>-97.82394153134501</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>STO 15%_Crisis</t>
+          <t>STO 15%_Recession</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1504,111 +1668,111 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Crisis (41%)</t>
+          <t>Recession (65%)</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>156576.5980458368</v>
+        <v>140495.7561256773</v>
       </c>
       <c r="E9" t="n">
-        <v>167496.3367301368</v>
+        <v>149716.8516460881</v>
       </c>
       <c r="F9" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>11477.75481791698</v>
+        <v>6124.744117516394</v>
       </c>
       <c r="H9" t="n">
-        <v>12798.5764749229</v>
+        <v>6816.358394385369</v>
       </c>
       <c r="I9" t="n">
-        <v>-145098.8432279198</v>
+        <v>-134371.012008161</v>
       </c>
       <c r="J9" t="n">
-        <v>-92.66955920542038</v>
+        <v>-95.64061984047572</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>STO 28%_Perfect</t>
+          <t>STO 15%_Crisis</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>STO 28%</t>
+          <t>STO 15%</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Perfect (100%)</t>
+          <t>Crisis (41%)</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>17395.12467039677</v>
+        <v>156402.8011420401</v>
       </c>
       <c r="E10" t="n">
-        <v>21038.2149648252</v>
+        <v>166524.1210733571</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="G10" t="n">
-        <v>323.2820483378213</v>
+        <v>11268.25091345382</v>
       </c>
       <c r="H10" t="n">
-        <v>365.8460643810284</v>
+        <v>12862.59784518622</v>
       </c>
       <c r="I10" t="n">
-        <v>-17071.84262205895</v>
+        <v>-145134.5502285863</v>
       </c>
       <c r="J10" t="n">
-        <v>-98.14153646804277</v>
+        <v>-92.7953650246837</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>STO 28%_Good</t>
+          <t>STO 15%_Extreme</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>STO 28%</t>
+          <t>STO 15%</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Good (84%)</t>
+          <t>Extreme (15%)</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>111465.1348523069</v>
+        <v>159597.0649230403</v>
       </c>
       <c r="E11" t="n">
-        <v>120002.435093471</v>
+        <v>168045.213339946</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="G11" t="n">
-        <v>2930.038027836275</v>
+        <v>11865.25870367696</v>
       </c>
       <c r="H11" t="n">
-        <v>3257.968593530237</v>
+        <v>13435.35185050296</v>
       </c>
       <c r="I11" t="n">
-        <v>-108535.0968244706</v>
+        <v>-147731.8062193634</v>
       </c>
       <c r="J11" t="n">
-        <v>-97.37134124341335</v>
+        <v>-92.56549065648636</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>STO 28%_Recession</t>
+          <t>STO 28%_Perfect</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1618,35 +1782,35 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Recession (65%)</t>
+          <t>Perfect (100%)</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>125142.6105336513</v>
+        <v>17154.89126112844</v>
       </c>
       <c r="E12" t="n">
-        <v>134675.7722791967</v>
+        <v>20601.66407879172</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>6315.191813822651</v>
+        <v>321.3932392963318</v>
       </c>
       <c r="H12" t="n">
-        <v>6957.46729829272</v>
+        <v>358.8113688117585</v>
       </c>
       <c r="I12" t="n">
-        <v>-118827.4187198286</v>
+        <v>-16833.4980218321</v>
       </c>
       <c r="J12" t="n">
-        <v>-94.9536039028653</v>
+        <v>-98.12652126787546</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>STO 28%_Crisis</t>
+          <t>STO 28%_Good</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1656,181 +1820,333 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Crisis (41%)</t>
+          <t>Good (84%)</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>143094.331373237</v>
+        <v>111529.9940324439</v>
       </c>
       <c r="E13" t="n">
-        <v>152803.629663798</v>
+        <v>120129.3880140484</v>
       </c>
       <c r="F13" t="n">
-        <v>196</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>11574.67257200867</v>
+        <v>2927.399515659442</v>
       </c>
       <c r="H13" t="n">
-        <v>12617.30770145806</v>
+        <v>3248.786017425488</v>
       </c>
       <c r="I13" t="n">
-        <v>-131519.6588012284</v>
+        <v>-108602.5945167844</v>
       </c>
       <c r="J13" t="n">
-        <v>-91.91115926051738</v>
+        <v>-97.3752356565106</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>STO 40%_Perfect</t>
+          <t>STO 28%_Recession</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>STO 40%</t>
+          <t>STO 28%</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Perfect (100%)</t>
+          <t>Recession (65%)</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>16948.71173573424</v>
+        <v>125263.9032285218</v>
       </c>
       <c r="E14" t="n">
-        <v>20564.07821330571</v>
+        <v>135025.4596369151</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>318.4910569569728</v>
+        <v>6360.415197846615</v>
       </c>
       <c r="H14" t="n">
-        <v>356.4227330958275</v>
+        <v>6962.65777981692</v>
       </c>
       <c r="I14" t="n">
-        <v>-16630.22067877727</v>
+        <v>-118903.4880306752</v>
       </c>
       <c r="J14" t="n">
-        <v>-98.12085389188917</v>
+        <v>-94.92238782768635</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>STO 40%_Good</t>
+          <t>STO 28%_Crisis</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>STO 40%</t>
+          <t>STO 28%</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Good (84%)</t>
+          <t>Crisis (41%)</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>98844.58605678441</v>
+        <v>143370.4323154436</v>
       </c>
       <c r="E15" t="n">
-        <v>107130.037330868</v>
+        <v>153551.0916585604</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="G15" t="n">
-        <v>3058.693908051168</v>
+        <v>11551.62508394768</v>
       </c>
       <c r="H15" t="n">
-        <v>3368.927032756765</v>
+        <v>12769.5051835566</v>
       </c>
       <c r="I15" t="n">
-        <v>-95785.89214873324</v>
+        <v>-131818.8072314959</v>
       </c>
       <c r="J15" t="n">
-        <v>-96.90555241306387</v>
+        <v>-91.94281212842283</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>STO 40%_Recession</t>
+          <t>STO 28%_Extreme</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>STO 40%</t>
+          <t>STO 28%</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Recession (65%)</t>
+          <t>Extreme (15%)</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>115089.4501373783</v>
+        <v>145775.4276440667</v>
       </c>
       <c r="E16" t="n">
-        <v>124018.9028566052</v>
+        <v>154961.0768302313</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="G16" t="n">
-        <v>6530.712254235763</v>
+        <v>11897.42073663007</v>
       </c>
       <c r="H16" t="n">
-        <v>7185.912309762005</v>
+        <v>13149.96385928181</v>
       </c>
       <c r="I16" t="n">
-        <v>-108558.7378831425</v>
+        <v>-133878.0069074366</v>
       </c>
       <c r="J16" t="n">
-        <v>-94.3255335337511</v>
+        <v>-91.83852798176694</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>STO 40%_Perfect</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Perfect (100%)</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>17438.78386417262</v>
+      </c>
+      <c r="E17" t="n">
+        <v>21352.25180847063</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>319.8245743840517</v>
+      </c>
+      <c r="H17" t="n">
+        <v>361.3372886141601</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-17118.95928978857</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-98.16601560707957</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>STO 40%_Good</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Good (84%)</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>97988.6364167962</v>
+      </c>
+      <c r="E18" t="n">
+        <v>107144.728420625</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3076.249359307586</v>
+      </c>
+      <c r="H18" t="n">
+        <v>3420.733179624282</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-94912.38705748861</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-96.86060601331086</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>STO 40%_Recession</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Recession (65%)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>113193.7073697877</v>
+      </c>
+      <c r="E19" t="n">
+        <v>123025.4694082533</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>6435.256177637727</v>
+      </c>
+      <c r="H19" t="n">
+        <v>7052.296749251489</v>
+      </c>
+      <c r="I19" t="n">
+        <v>-106758.45119215</v>
+      </c>
+      <c r="J19" t="n">
+        <v>-94.31482868865257</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>STO 40%_Crisis</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>STO 40%</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>Crisis (41%)</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>131034.2677424282</v>
-      </c>
-      <c r="E17" t="n">
-        <v>141460.4748809713</v>
-      </c>
-      <c r="F17" t="n">
-        <v>262.3431219818424</v>
-      </c>
-      <c r="G17" t="n">
-        <v>11643.08994277793</v>
-      </c>
-      <c r="H17" t="n">
-        <v>12674.35080814071</v>
-      </c>
-      <c r="I17" t="n">
-        <v>-119391.1777996503</v>
-      </c>
-      <c r="J17" t="n">
-        <v>-91.11446941065481</v>
+      <c r="D20" t="n">
+        <v>131654.3383120974</v>
+      </c>
+      <c r="E20" t="n">
+        <v>142258.0594928669</v>
+      </c>
+      <c r="F20" t="n">
+        <v>180.2404020138272</v>
+      </c>
+      <c r="G20" t="n">
+        <v>11578.83426462438</v>
+      </c>
+      <c r="H20" t="n">
+        <v>12781.13345433567</v>
+      </c>
+      <c r="I20" t="n">
+        <v>-120075.504047473</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-91.20512516862466</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>STO 40%_Extreme</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Extreme (15%)</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>135250.7601474534</v>
+      </c>
+      <c r="E21" t="n">
+        <v>145073.068370846</v>
+      </c>
+      <c r="F21" t="n">
+        <v>280</v>
+      </c>
+      <c r="G21" t="n">
+        <v>11921.55368899196</v>
+      </c>
+      <c r="H21" t="n">
+        <v>13063.49037561235</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-123329.2064584615</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-91.18559209870996</v>
       </c>
     </row>
   </sheetData>
@@ -1844,7 +2160,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1896,16 +2212,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>121489.4720318987</v>
+        <v>121829.664114389</v>
       </c>
       <c r="D2" t="n">
-        <v>17233.06405730591</v>
+        <v>17945.48087318345</v>
       </c>
       <c r="E2" t="n">
-        <v>104256.4079745928</v>
+        <v>103884.1832412056</v>
       </c>
       <c r="F2" t="n">
-        <v>85.81517906935909</v>
+        <v>85.27002351715099</v>
       </c>
     </row>
     <row r="3">
@@ -1920,16 +2236,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>121489.4720318987</v>
+        <v>121829.664114389</v>
       </c>
       <c r="D3" t="n">
-        <v>17395.12467039677</v>
+        <v>17154.89126112844</v>
       </c>
       <c r="E3" t="n">
-        <v>104094.3473615019</v>
+        <v>104674.7728532606</v>
       </c>
       <c r="F3" t="n">
-        <v>85.68178429005812</v>
+        <v>85.91895382308429</v>
       </c>
     </row>
     <row r="4">
@@ -1944,16 +2260,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>121489.4720318987</v>
+        <v>121829.664114389</v>
       </c>
       <c r="D4" t="n">
-        <v>16948.71173573424</v>
+        <v>17438.78386417262</v>
       </c>
       <c r="E4" t="n">
-        <v>104540.7602961645</v>
+        <v>104390.8802502164</v>
       </c>
       <c r="F4" t="n">
-        <v>86.04923418279066</v>
+        <v>85.6859296207212</v>
       </c>
     </row>
     <row r="5">
@@ -1968,16 +2284,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>186233.2080458938</v>
+        <v>187893.2467576699</v>
       </c>
       <c r="D5" t="n">
-        <v>127259.3429977431</v>
+        <v>126819.6940210681</v>
       </c>
       <c r="E5" t="n">
-        <v>58973.86504815078</v>
+        <v>61073.55273660182</v>
       </c>
       <c r="F5" t="n">
-        <v>31.66667516870446</v>
+        <v>32.50438948206038</v>
       </c>
     </row>
     <row r="6">
@@ -1992,16 +2308,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>186233.2080458938</v>
+        <v>187893.2467576699</v>
       </c>
       <c r="D6" t="n">
-        <v>111465.1348523069</v>
+        <v>111529.9940324439</v>
       </c>
       <c r="E6" t="n">
-        <v>74768.07319358693</v>
+        <v>76363.25272522605</v>
       </c>
       <c r="F6" t="n">
-        <v>40.14755154470714</v>
+        <v>40.64182935947316</v>
       </c>
     </row>
     <row r="7">
@@ -2016,16 +2332,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>186233.2080458938</v>
+        <v>187893.2467576699</v>
       </c>
       <c r="D7" t="n">
-        <v>98844.58605678441</v>
+        <v>97988.6364167962</v>
       </c>
       <c r="E7" t="n">
-        <v>87388.62198910944</v>
+        <v>89904.61034087373</v>
       </c>
       <c r="F7" t="n">
-        <v>46.92429610489987</v>
+        <v>47.84877151908801</v>
       </c>
     </row>
     <row r="8">
@@ -2040,16 +2356,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>199551.9300674134</v>
+        <v>198985.6758993856</v>
       </c>
       <c r="D8" t="n">
-        <v>139668.8077281435</v>
+        <v>140495.7561256773</v>
       </c>
       <c r="E8" t="n">
-        <v>59883.12233926993</v>
+        <v>58489.91977370824</v>
       </c>
       <c r="F8" t="n">
-        <v>30.00879135523269</v>
+        <v>29.39403527884232</v>
       </c>
     </row>
     <row r="9">
@@ -2064,16 +2380,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>199551.9300674134</v>
+        <v>198985.6758993856</v>
       </c>
       <c r="D9" t="n">
-        <v>125142.6105336513</v>
+        <v>125263.9032285218</v>
       </c>
       <c r="E9" t="n">
-        <v>74409.31953376214</v>
+        <v>73721.77267086379</v>
       </c>
       <c r="F9" t="n">
-        <v>37.28819836952963</v>
+        <v>37.04878370649162</v>
       </c>
     </row>
     <row r="10">
@@ -2088,16 +2404,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>199551.9300674134</v>
+        <v>198985.6758993856</v>
       </c>
       <c r="D10" t="n">
-        <v>115089.4501373783</v>
+        <v>113193.7073697877</v>
       </c>
       <c r="E10" t="n">
-        <v>84462.47993003512</v>
+        <v>85791.96852959789</v>
       </c>
       <c r="F10" t="n">
-        <v>42.32606515081146</v>
+        <v>43.1146453843127</v>
       </c>
     </row>
     <row r="11">
@@ -2112,16 +2428,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>209997.9724065157</v>
+        <v>211240.7588842058</v>
       </c>
       <c r="D11" t="n">
-        <v>156576.5980458368</v>
+        <v>156402.8011420401</v>
       </c>
       <c r="E11" t="n">
-        <v>53421.37436067889</v>
+        <v>54837.95774216572</v>
       </c>
       <c r="F11" t="n">
-        <v>25.43899531432874</v>
+        <v>25.95993217967267</v>
       </c>
     </row>
     <row r="12">
@@ -2136,16 +2452,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>209997.9724065157</v>
+        <v>211240.7588842058</v>
       </c>
       <c r="D12" t="n">
-        <v>143094.331373237</v>
+        <v>143370.4323154436</v>
       </c>
       <c r="E12" t="n">
-        <v>66903.64103327869</v>
+        <v>67870.32656876228</v>
       </c>
       <c r="F12" t="n">
-        <v>31.859184289535</v>
+        <v>32.12937073662295</v>
       </c>
     </row>
     <row r="13">
@@ -2160,16 +2476,88 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>209997.9724065157</v>
+        <v>211240.7588842058</v>
       </c>
       <c r="D13" t="n">
-        <v>131034.2677424282</v>
+        <v>131654.3383120974</v>
       </c>
       <c r="E13" t="n">
-        <v>78963.70466408746</v>
+        <v>79586.42057210841</v>
       </c>
       <c r="F13" t="n">
-        <v>37.60212718208007</v>
+        <v>37.67569336168437</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Extreme (15%)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>STO 15%</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>211331.4606634509</v>
+      </c>
+      <c r="D14" t="n">
+        <v>159597.0649230403</v>
+      </c>
+      <c r="E14" t="n">
+        <v>51734.3957404106</v>
+      </c>
+      <c r="F14" t="n">
+        <v>24.48021490884338</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Extreme (15%)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>STO 28%</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>211331.4606634509</v>
+      </c>
+      <c r="D15" t="n">
+        <v>145775.4276440667</v>
+      </c>
+      <c r="E15" t="n">
+        <v>65556.03301938419</v>
+      </c>
+      <c r="F15" t="n">
+        <v>31.02047977787052</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Extreme (15%)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>211331.4606634509</v>
+      </c>
+      <c r="D16" t="n">
+        <v>135250.7601474534</v>
+      </c>
+      <c r="E16" t="n">
+        <v>76080.70051599748</v>
+      </c>
+      <c r="F16" t="n">
+        <v>36.0006504839132</v>
       </c>
     </row>
   </sheetData>
@@ -2183,7 +2571,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2250,7 +2638,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.9823143022526057</v>
+        <v>0.9822986308332026</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -2282,19 +2670,19 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.81875756094707</v>
+        <v>0.8186366174467081</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0001010327839969894</v>
+        <v>7.707580972188864e-05</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0001010327839969894</v>
+        <v>7.707580972188864e-05</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0152</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="4">
@@ -2314,19 +2702,19 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.6416063235468267</v>
+        <v>0.6416906222967823</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0005745609146250596</v>
+        <v>0.0006071513183129611</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0005745609146250596</v>
+        <v>0.0006071513183129611</v>
       </c>
       <c r="H4" t="n">
-        <v>0.041</v>
+        <v>0.0382</v>
       </c>
     </row>
     <row r="5">
@@ -2346,57 +2734,57 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.4136345003583995</v>
+        <v>0.413327534293121</v>
       </c>
       <c r="E5" t="n">
         <v>0.009999999999999905</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02320890123150835</v>
+        <v>0.02749445546428887</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01320890123150845</v>
+        <v>0.01749445546428896</v>
       </c>
       <c r="H5" t="n">
-        <v>0.06419999999999999</v>
+        <v>0.064</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>STO 28%_Perfect</t>
+          <t>STO 15%_Extreme</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>STO 28%</t>
+          <t>STO 15%</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Perfect (100%)</t>
+          <t>Extreme (15%)</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.982289528511714</v>
+        <v>0.3967631143114563</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.009999999999999905</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.02485180089578153</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.01485180089578163</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.07920000000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>STO 28%_Good</t>
+          <t>STO 28%_Perfect</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2406,29 +2794,29 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Good (84%)</t>
+          <t>Perfect (100%)</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.8169322596973189</v>
+        <v>0.9823196459810106</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>4.535532507098437e-05</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>4.535532507098437e-05</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0118</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>STO 28%_Recession</t>
+          <t>STO 28%_Good</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2438,29 +2826,29 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Recession (65%)</t>
+          <t>Good (84%)</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.6390038704741831</v>
+        <v>0.8171811642575961</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0005201782828060917</v>
+        <v>5.912561875968674e-05</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0005201782828060917</v>
+        <v>5.912561875968674e-05</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0442</v>
+        <v>0.0132</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>STO 28%_Crisis</t>
+          <t>STO 28%_Recession</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2470,93 +2858,93 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Crisis (41%)</t>
+          <t>Recession (65%)</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.4132660348296509</v>
+        <v>0.6396710372473863</v>
       </c>
       <c r="E9" t="n">
-        <v>0.00999999999999995</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0234222611596614</v>
+        <v>0.000555384797919084</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01342226115966145</v>
+        <v>0.000555384797919084</v>
       </c>
       <c r="H9" t="n">
-        <v>0.064</v>
+        <v>0.0446</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>STO 40%_Perfect</t>
+          <t>STO 28%_Crisis</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>STO 40%</t>
+          <t>STO 28%</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Perfect (100%)</t>
+          <t>Crisis (41%)</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.9823121013038794</v>
+        <v>0.4119103335077707</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>0.00999999999999995</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.02489130257355281</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.01489130257355286</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.0608</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>STO 40%_Good</t>
+          <t>STO 28%_Extreme</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>STO 40%</t>
+          <t>STO 28%</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Good (84%)</t>
+          <t>Extreme (15%)</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.8155323903846202</v>
+        <v>0.3939539599978985</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.00999999999999995</v>
       </c>
       <c r="F11" t="n">
-        <v>5.003315759281891e-05</v>
+        <v>0.02332944757897115</v>
       </c>
       <c r="G11" t="n">
-        <v>5.003315759281891e-05</v>
+        <v>0.0133294475789712</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0156</v>
+        <v>0.07779999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>STO 40%_Recession</t>
+          <t>STO 40%_Perfect</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2566,55 +2954,151 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Recession (65%)</t>
+          <t>Perfect (100%)</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.6368769188635667</v>
+        <v>0.9823392407637377</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.000422501511520011</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.000422501511520011</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0384</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>STO 40%_Good</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Good (84%)</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.8154540468899483</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5.212294998329787e-05</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5.212294998329787e-05</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.0164</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>STO 40%_Recession</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Recession (65%)</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.637036077665824</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0004304157314349371</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0004304157314349371</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0402</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>STO 40%_Crisis</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>STO 40%</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Crisis (41%)</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>0.4094635588208302</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.009369397213637195</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.02533414121601242</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.01596474400237523</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.0636</v>
+      <c r="D15" t="n">
+        <v>0.4112745638097692</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.006437157214779519</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.02494204968688549</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.01850489247210597</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0602</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>STO 40%_Extreme</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>STO 40%</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Extreme (15%)</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.3921787635140916</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.009999999999999966</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.02361353547521183</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.01361353547521187</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.07580000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>